<commit_message>
Log4j2 Properties File Added
</commit_message>
<xml_diff>
--- a/TestDatas/TutorialsNinja.xlsx
+++ b/TestDatas/TutorialsNinja.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59E63A0-ACA0-455D-BDFA-87714F05355B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{19A1EE90-E006-4BA0-A3A8-1BF5CDA9EA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J18"/>
 </workbook>
 </file>
 
@@ -718,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -771,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>